<commit_message>
Finished 1cm curvature analysis for 2015
</commit_message>
<xml_diff>
--- a/data/GIS_MPQ_Analysis_1cm_Curvature.xlsx
+++ b/data/GIS_MPQ_Analysis_1cm_Curvature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23900" yWindow="1280" windowWidth="25600" windowHeight="11680" tabRatio="500"/>
+    <workbookView xWindow="27640" yWindow="1320" windowWidth="21780" windowHeight="11680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Curvature" sheetId="2" r:id="rId1"/>
@@ -126,8 +126,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -148,7 +206,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -156,6 +214,35 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -163,6 +250,35 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -836,6 +952,27 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
+      <c r="D11">
+        <v>199289</v>
+      </c>
+      <c r="E11">
+        <v>19.928899999999999</v>
+      </c>
+      <c r="F11">
+        <v>-664256.3125</v>
+      </c>
+      <c r="G11">
+        <v>1001988.4375</v>
+      </c>
+      <c r="H11">
+        <v>1666244.75</v>
+      </c>
+      <c r="I11">
+        <v>2.3879000000000001</v>
+      </c>
+      <c r="J11">
+        <v>26487.705945000002</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
@@ -847,6 +984,27 @@
       <c r="C12" t="s">
         <v>6</v>
       </c>
+      <c r="D12">
+        <v>211455</v>
+      </c>
+      <c r="E12">
+        <v>21.145499999999998</v>
+      </c>
+      <c r="F12">
+        <v>-586815.8125</v>
+      </c>
+      <c r="G12">
+        <v>567830.8125</v>
+      </c>
+      <c r="H12">
+        <v>1154646.625</v>
+      </c>
+      <c r="I12">
+        <v>-1.883634</v>
+      </c>
+      <c r="J12">
+        <v>21791.173404000001</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
@@ -954,8 +1112,29 @@
       <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>198986</v>
+      </c>
+      <c r="E16">
+        <v>19.898599999999998</v>
+      </c>
+      <c r="F16">
+        <v>-1218061.5</v>
+      </c>
+      <c r="G16">
+        <v>995438.5625</v>
+      </c>
+      <c r="H16">
+        <v>2213500.0625</v>
+      </c>
+      <c r="I16">
+        <v>12.212949999999999</v>
+      </c>
+      <c r="J16">
+        <v>40244.563208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -965,8 +1144,29 @@
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>200797</v>
+      </c>
+      <c r="E17">
+        <v>20.079699999999999</v>
+      </c>
+      <c r="F17">
+        <v>-581158.375</v>
+      </c>
+      <c r="G17">
+        <v>413679.125</v>
+      </c>
+      <c r="H17">
+        <v>994837.5</v>
+      </c>
+      <c r="I17">
+        <v>-0.26499499999999998</v>
+      </c>
+      <c r="J17">
+        <v>25144.194873</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -976,8 +1176,29 @@
       <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>145188</v>
+      </c>
+      <c r="E18">
+        <v>14.518800000000001</v>
+      </c>
+      <c r="F18">
+        <v>-484825.625</v>
+      </c>
+      <c r="G18">
+        <v>404021.5</v>
+      </c>
+      <c r="H18">
+        <v>888847.125</v>
+      </c>
+      <c r="I18">
+        <v>-0.469748</v>
+      </c>
+      <c r="J18">
+        <v>22543.819511999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -987,8 +1208,29 @@
       <c r="C19" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>174691</v>
+      </c>
+      <c r="E19">
+        <v>17.469100000000001</v>
+      </c>
+      <c r="F19">
+        <v>-1193695.25</v>
+      </c>
+      <c r="G19">
+        <v>827917.3125</v>
+      </c>
+      <c r="H19">
+        <v>2021612.5625</v>
+      </c>
+      <c r="I19">
+        <v>-6.6086020000000003</v>
+      </c>
+      <c r="J19">
+        <v>39218.805068000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -998,8 +1240,29 @@
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>169500</v>
+      </c>
+      <c r="E20">
+        <v>16.95</v>
+      </c>
+      <c r="F20">
+        <v>-644506.1875</v>
+      </c>
+      <c r="G20">
+        <v>1012788.5625</v>
+      </c>
+      <c r="H20">
+        <v>1657294.75</v>
+      </c>
+      <c r="I20">
+        <v>19.026001999999998</v>
+      </c>
+      <c r="J20">
+        <v>33495.219247000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1009,8 +1272,29 @@
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <v>192603</v>
+      </c>
+      <c r="E21">
+        <v>19.260300000000001</v>
+      </c>
+      <c r="F21">
+        <v>-1068989.75</v>
+      </c>
+      <c r="G21">
+        <v>1191166.125</v>
+      </c>
+      <c r="H21">
+        <v>2260155.875</v>
+      </c>
+      <c r="I21">
+        <v>26.881910000000001</v>
+      </c>
+      <c r="J21">
+        <v>40179.384750999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1020,8 +1304,29 @@
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>167522</v>
+      </c>
+      <c r="E22">
+        <v>16.752199999999998</v>
+      </c>
+      <c r="F22">
+        <v>-695221.4375</v>
+      </c>
+      <c r="G22">
+        <v>917453.5</v>
+      </c>
+      <c r="H22">
+        <v>1612674.9375</v>
+      </c>
+      <c r="I22">
+        <v>23.340506000000001</v>
+      </c>
+      <c r="J22">
+        <v>28921.363394</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1031,8 +1336,29 @@
       <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <v>178577</v>
+      </c>
+      <c r="E23">
+        <v>17.857700000000001</v>
+      </c>
+      <c r="F23">
+        <v>-1371410.625</v>
+      </c>
+      <c r="G23">
+        <v>1016936.8125</v>
+      </c>
+      <c r="H23">
+        <v>2388347.4375</v>
+      </c>
+      <c r="I23">
+        <v>29.830068000000001</v>
+      </c>
+      <c r="J23">
+        <v>47951.082281000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1041,6 +1367,27 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="D24">
+        <v>169602</v>
+      </c>
+      <c r="E24">
+        <v>16.9602</v>
+      </c>
+      <c r="F24">
+        <v>-1753387.875</v>
+      </c>
+      <c r="G24">
+        <v>1206146.5</v>
+      </c>
+      <c r="H24">
+        <v>2959534.375</v>
+      </c>
+      <c r="I24">
+        <v>28.063424000000001</v>
+      </c>
+      <c r="J24">
+        <v>55525.653897999997</v>
       </c>
     </row>
   </sheetData>
@@ -1058,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1400,6 +1747,27 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
+      <c r="D11">
+        <v>199289</v>
+      </c>
+      <c r="E11">
+        <v>19.928899999999999</v>
+      </c>
+      <c r="F11">
+        <v>-419792.15625</v>
+      </c>
+      <c r="G11">
+        <v>451373.96875</v>
+      </c>
+      <c r="H11">
+        <v>871166.125</v>
+      </c>
+      <c r="I11">
+        <v>212.855861</v>
+      </c>
+      <c r="J11">
+        <v>9837.8624120000004</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
@@ -1411,6 +1779,27 @@
       <c r="C12" t="s">
         <v>6</v>
       </c>
+      <c r="D12">
+        <v>211455</v>
+      </c>
+      <c r="E12">
+        <v>21.145499999999998</v>
+      </c>
+      <c r="F12">
+        <v>-288059.4375</v>
+      </c>
+      <c r="G12">
+        <v>286990.59375</v>
+      </c>
+      <c r="H12">
+        <v>575050.03125</v>
+      </c>
+      <c r="I12">
+        <v>230.774946</v>
+      </c>
+      <c r="J12">
+        <v>8169.9046719999997</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
@@ -1518,8 +1907,29 @@
       <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>198986</v>
+      </c>
+      <c r="E16">
+        <v>19.898599999999998</v>
+      </c>
+      <c r="F16">
+        <v>-830920.625</v>
+      </c>
+      <c r="G16">
+        <v>726528.125</v>
+      </c>
+      <c r="H16">
+        <v>1557448.75</v>
+      </c>
+      <c r="I16">
+        <v>-69.965064999999996</v>
+      </c>
+      <c r="J16">
+        <v>17108.019038999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1529,8 +1939,29 @@
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>200797</v>
+      </c>
+      <c r="E17">
+        <v>20.079699999999999</v>
+      </c>
+      <c r="F17">
+        <v>-291865.3125</v>
+      </c>
+      <c r="G17">
+        <v>260779.40625</v>
+      </c>
+      <c r="H17">
+        <v>552644.71875</v>
+      </c>
+      <c r="I17">
+        <v>157.47254000000001</v>
+      </c>
+      <c r="J17">
+        <v>10253.25049</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1540,8 +1971,29 @@
       <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>145188</v>
+      </c>
+      <c r="E18">
+        <v>14.518800000000001</v>
+      </c>
+      <c r="F18">
+        <v>-318155.125</v>
+      </c>
+      <c r="G18">
+        <v>222519.671875</v>
+      </c>
+      <c r="H18">
+        <v>540674.796875</v>
+      </c>
+      <c r="I18">
+        <v>185.58637899999999</v>
+      </c>
+      <c r="J18">
+        <v>8946.3652750000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1551,8 +2003,29 @@
       <c r="C19" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>174691</v>
+      </c>
+      <c r="E19">
+        <v>17.469100000000001</v>
+      </c>
+      <c r="F19">
+        <v>-605731.1875</v>
+      </c>
+      <c r="G19">
+        <v>660538.875</v>
+      </c>
+      <c r="H19">
+        <v>1266270.0625</v>
+      </c>
+      <c r="I19">
+        <v>53.949736999999999</v>
+      </c>
+      <c r="J19">
+        <v>16757.179501999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1562,8 +2035,29 @@
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>169500</v>
+      </c>
+      <c r="E20">
+        <v>16.95</v>
+      </c>
+      <c r="F20">
+        <v>-415213.46875</v>
+      </c>
+      <c r="G20">
+        <v>464095.25</v>
+      </c>
+      <c r="H20">
+        <v>879308.71875</v>
+      </c>
+      <c r="I20">
+        <v>106.362432</v>
+      </c>
+      <c r="J20">
+        <v>14234.795894000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1573,8 +2067,29 @@
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <v>192603</v>
+      </c>
+      <c r="E21">
+        <v>19.260300000000001</v>
+      </c>
+      <c r="F21">
+        <v>-684005.6875</v>
+      </c>
+      <c r="G21">
+        <v>771900.5</v>
+      </c>
+      <c r="H21">
+        <v>1455906.1875</v>
+      </c>
+      <c r="I21">
+        <v>134.78174899999999</v>
+      </c>
+      <c r="J21">
+        <v>18250.686593999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1584,8 +2099,29 @@
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>167522</v>
+      </c>
+      <c r="E22">
+        <v>16.752199999999998</v>
+      </c>
+      <c r="F22">
+        <v>-357413</v>
+      </c>
+      <c r="G22">
+        <v>612217.875</v>
+      </c>
+      <c r="H22">
+        <v>969630.875</v>
+      </c>
+      <c r="I22">
+        <v>132.65367800000001</v>
+      </c>
+      <c r="J22">
+        <v>11332.558585000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1595,8 +2131,29 @@
       <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <v>178577</v>
+      </c>
+      <c r="E23">
+        <v>17.857700000000001</v>
+      </c>
+      <c r="F23">
+        <v>-688331.4375</v>
+      </c>
+      <c r="G23">
+        <v>683380.8125</v>
+      </c>
+      <c r="H23">
+        <v>1371712.25</v>
+      </c>
+      <c r="I23">
+        <v>98.673505000000006</v>
+      </c>
+      <c r="J23">
+        <v>21115.616704</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1605,6 +2162,27 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="D24">
+        <v>169602</v>
+      </c>
+      <c r="E24">
+        <v>16.9602</v>
+      </c>
+      <c r="F24">
+        <v>-1199566.25</v>
+      </c>
+      <c r="G24">
+        <v>605247.5625</v>
+      </c>
+      <c r="H24">
+        <v>1804813.8125</v>
+      </c>
+      <c r="I24">
+        <v>-175.33552499999999</v>
+      </c>
+      <c r="J24">
+        <v>25211.843893000001</v>
       </c>
     </row>
   </sheetData>
@@ -1622,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1964,6 +2542,27 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
+      <c r="D11">
+        <v>199289</v>
+      </c>
+      <c r="E11">
+        <v>19.928899999999999</v>
+      </c>
+      <c r="F11">
+        <v>-550614.4375</v>
+      </c>
+      <c r="G11">
+        <v>407756.6875</v>
+      </c>
+      <c r="H11">
+        <v>958371.125</v>
+      </c>
+      <c r="I11">
+        <v>210.46795900000001</v>
+      </c>
+      <c r="J11">
+        <v>19999.705773000001</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
@@ -1975,6 +2574,27 @@
       <c r="C12" t="s">
         <v>6</v>
       </c>
+      <c r="D12">
+        <v>211455</v>
+      </c>
+      <c r="E12">
+        <v>21.145499999999998</v>
+      </c>
+      <c r="F12">
+        <v>-347450.6875</v>
+      </c>
+      <c r="G12">
+        <v>337081.84375</v>
+      </c>
+      <c r="H12">
+        <v>684532.53125</v>
+      </c>
+      <c r="I12">
+        <v>232.65858299999999</v>
+      </c>
+      <c r="J12">
+        <v>16397.700195000001</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
@@ -2082,8 +2702,29 @@
       <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>198986</v>
+      </c>
+      <c r="E16">
+        <v>19.898599999999998</v>
+      </c>
+      <c r="F16">
+        <v>-609494.8125</v>
+      </c>
+      <c r="G16">
+        <v>551443.5625</v>
+      </c>
+      <c r="H16">
+        <v>1160938.375</v>
+      </c>
+      <c r="I16">
+        <v>-82.178014000000005</v>
+      </c>
+      <c r="J16">
+        <v>28786.213066</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2093,8 +2734,29 @@
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>200797</v>
+      </c>
+      <c r="E17">
+        <v>20.079699999999999</v>
+      </c>
+      <c r="F17">
+        <v>-251671.375</v>
+      </c>
+      <c r="G17">
+        <v>289293.09375</v>
+      </c>
+      <c r="H17">
+        <v>540964.46875</v>
+      </c>
+      <c r="I17">
+        <v>157.737538</v>
+      </c>
+      <c r="J17">
+        <v>18279.826574999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -2104,8 +2766,29 @@
       <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>145188</v>
+      </c>
+      <c r="E18">
+        <v>14.518800000000001</v>
+      </c>
+      <c r="F18">
+        <v>-222949.421875</v>
+      </c>
+      <c r="G18">
+        <v>251741.09375</v>
+      </c>
+      <c r="H18">
+        <v>474690.515625</v>
+      </c>
+      <c r="I18">
+        <v>186.05612500000001</v>
+      </c>
+      <c r="J18">
+        <v>16572.217178999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2115,8 +2798,29 @@
       <c r="C19" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>174691</v>
+      </c>
+      <c r="E19">
+        <v>17.469100000000001</v>
+      </c>
+      <c r="F19">
+        <v>-500761.0625</v>
+      </c>
+      <c r="G19">
+        <v>587964.125</v>
+      </c>
+      <c r="H19">
+        <v>1088725.1875</v>
+      </c>
+      <c r="I19">
+        <v>60.558332999999998</v>
+      </c>
+      <c r="J19">
+        <v>27800.070318999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2126,8 +2830,29 @@
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>169500</v>
+      </c>
+      <c r="E20">
+        <v>16.95</v>
+      </c>
+      <c r="F20">
+        <v>-548693.25</v>
+      </c>
+      <c r="G20">
+        <v>434067.4375</v>
+      </c>
+      <c r="H20">
+        <v>982760.6875</v>
+      </c>
+      <c r="I20">
+        <v>87.336432000000002</v>
+      </c>
+      <c r="J20">
+        <v>23643.288209999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2137,8 +2862,29 @@
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <v>192603</v>
+      </c>
+      <c r="E21">
+        <v>19.260300000000001</v>
+      </c>
+      <c r="F21">
+        <v>-560219.75</v>
+      </c>
+      <c r="G21">
+        <v>470533.84375</v>
+      </c>
+      <c r="H21">
+        <v>1030753.59375</v>
+      </c>
+      <c r="I21">
+        <v>107.89984200000001</v>
+      </c>
+      <c r="J21">
+        <v>27445.876854999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2148,8 +2894,29 @@
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>167522</v>
+      </c>
+      <c r="E22">
+        <v>16.752199999999998</v>
+      </c>
+      <c r="F22">
+        <v>-604190.75</v>
+      </c>
+      <c r="G22">
+        <v>363408.75</v>
+      </c>
+      <c r="H22">
+        <v>967599.5</v>
+      </c>
+      <c r="I22">
+        <v>109.31317</v>
+      </c>
+      <c r="J22">
+        <v>21393.328504000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2159,8 +2926,29 @@
       <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <v>178577</v>
+      </c>
+      <c r="E23">
+        <v>17.857700000000001</v>
+      </c>
+      <c r="F23">
+        <v>-473871.96875</v>
+      </c>
+      <c r="G23">
+        <v>683079.1875</v>
+      </c>
+      <c r="H23">
+        <v>1156951.15625</v>
+      </c>
+      <c r="I23">
+        <v>68.843442999999994</v>
+      </c>
+      <c r="J23">
+        <v>32973.437319999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2169,6 +2957,27 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="D24">
+        <v>169602</v>
+      </c>
+      <c r="E24">
+        <v>16.9602</v>
+      </c>
+      <c r="F24">
+        <v>-669846.0625</v>
+      </c>
+      <c r="G24">
+        <v>1069074</v>
+      </c>
+      <c r="H24">
+        <v>1738920.0625</v>
+      </c>
+      <c r="I24">
+        <v>-203.39894000000001</v>
+      </c>
+      <c r="J24">
+        <v>37925.557688000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 2015 curvature values with clip method
</commit_message>
<xml_diff>
--- a/data/GIS_MPQ_Analysis_1cm_Curvature.xlsx
+++ b/data/GIS_MPQ_Analysis_1cm_Curvature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27640" yWindow="1320" windowWidth="21780" windowHeight="11680" tabRatio="500"/>
+    <workbookView xWindow="28560" yWindow="1980" windowWidth="21780" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Curvature" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="294">
   <si>
     <t>Field_Season</t>
   </si>
@@ -63,6 +63,846 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>MIN_CLIP</t>
+  </si>
+  <si>
+    <t>MAX_CLIP</t>
+  </si>
+  <si>
+    <t>MEAN_CLIP</t>
+  </si>
+  <si>
+    <t>STD_CLIP</t>
+  </si>
+  <si>
+    <t>﻿-1519387.5</t>
+  </si>
+  <si>
+    <t>﻿1175441.75</t>
+  </si>
+  <si>
+    <t>﻿-20.3835249951077</t>
+  </si>
+  <si>
+    <t>﻿72470.51109052158</t>
+  </si>
+  <si>
+    <t>﻿-959136.25</t>
+  </si>
+  <si>
+    <t>﻿979291.0625</t>
+  </si>
+  <si>
+    <t>﻿-652.558912196695</t>
+  </si>
+  <si>
+    <t>﻿33416.5182919773</t>
+  </si>
+  <si>
+    <t>﻿-607051.3125</t>
+  </si>
+  <si>
+    <t>﻿740197</t>
+  </si>
+  <si>
+    <t>﻿-632.1753834566168</t>
+  </si>
+  <si>
+    <t>﻿48355.09423347204</t>
+  </si>
+  <si>
+    <t>﻿-1859189.375</t>
+  </si>
+  <si>
+    <t>﻿1205290.375</t>
+  </si>
+  <si>
+    <t>﻿-4.007588525752517</t>
+  </si>
+  <si>
+    <t>﻿71827.22941424637</t>
+  </si>
+  <si>
+    <t>﻿-941427.375</t>
+  </si>
+  <si>
+    <t>﻿826234.0625</t>
+  </si>
+  <si>
+    <t>﻿-484.4054215426426</t>
+  </si>
+  <si>
+    <t>﻿31855.6996400756</t>
+  </si>
+  <si>
+    <t>﻿-763117.875</t>
+  </si>
+  <si>
+    <t>﻿917762</t>
+  </si>
+  <si>
+    <t>﻿-480.3978313135146</t>
+  </si>
+  <si>
+    <t>﻿47897.28402973769</t>
+  </si>
+  <si>
+    <t>﻿-994112.9375</t>
+  </si>
+  <si>
+    <t>﻿1093561.125</t>
+  </si>
+  <si>
+    <t>﻿14.76181025570984</t>
+  </si>
+  <si>
+    <t>﻿32112.457613948</t>
+  </si>
+  <si>
+    <t>﻿-500548.15625</t>
+  </si>
+  <si>
+    <t>﻿576804.5625</t>
+  </si>
+  <si>
+    <t>﻿260.6243394192841</t>
+  </si>
+  <si>
+    <t>﻿12796.57179616994</t>
+  </si>
+  <si>
+    <t>﻿-525422</t>
+  </si>
+  <si>
+    <t>﻿532709.25</t>
+  </si>
+  <si>
+    <t>﻿245.8625279660764</t>
+  </si>
+  <si>
+    <t>﻿23473.09005405265</t>
+  </si>
+  <si>
+    <t>﻿-664256.3125</t>
+  </si>
+  <si>
+    <t>﻿1001988.4375</t>
+  </si>
+  <si>
+    <t>﻿4.447495424251402</t>
+  </si>
+  <si>
+    <t>﻿26476.02507113626</t>
+  </si>
+  <si>
+    <t>﻿-419792.15625</t>
+  </si>
+  <si>
+    <t>﻿451373.96875</t>
+  </si>
+  <si>
+    <t>﻿213.5568866714697</t>
+  </si>
+  <si>
+    <t>﻿9835.527894504296</t>
+  </si>
+  <si>
+    <t>﻿-550614.4375</t>
+  </si>
+  <si>
+    <t>﻿407756.6875</t>
+  </si>
+  <si>
+    <t>﻿209.1093893721227</t>
+  </si>
+  <si>
+    <t>﻿19991.51264015555</t>
+  </si>
+  <si>
+    <t>﻿-586815.8125</t>
+  </si>
+  <si>
+    <t>﻿567830.8125</t>
+  </si>
+  <si>
+    <t>﻿-4.831450825958506</t>
+  </si>
+  <si>
+    <t>﻿21781.15938683151</t>
+  </si>
+  <si>
+    <t>﻿-288059.4375</t>
+  </si>
+  <si>
+    <t>﻿286990.59375</t>
+  </si>
+  <si>
+    <t>﻿229.2795172002806</t>
+  </si>
+  <si>
+    <t>﻿8163.497539129872</t>
+  </si>
+  <si>
+    <t>﻿-347450.6875</t>
+  </si>
+  <si>
+    <t>﻿337081.84375</t>
+  </si>
+  <si>
+    <t>﻿234.1109702350115</t>
+  </si>
+  <si>
+    <t>﻿16394.15356175459</t>
+  </si>
+  <si>
+    <t>﻿-2364842.5</t>
+  </si>
+  <si>
+    <t>﻿2575248.5</t>
+  </si>
+  <si>
+    <t>﻿10.77765757379625</t>
+  </si>
+  <si>
+    <t>﻿136726.3808772916</t>
+  </si>
+  <si>
+    <t>﻿-1281191.5</t>
+  </si>
+  <si>
+    <t>﻿1371673.375</t>
+  </si>
+  <si>
+    <t>﻿-1269.360717663153</t>
+  </si>
+  <si>
+    <t>﻿70823.61489212977</t>
+  </si>
+  <si>
+    <t>﻿-1590550.25</t>
+  </si>
+  <si>
+    <t>﻿1195325.125</t>
+  </si>
+  <si>
+    <t>﻿-1280.138385578402</t>
+  </si>
+  <si>
+    <t>﻿81315.6246247527</t>
+  </si>
+  <si>
+    <t>﻿-1816623.875</t>
+  </si>
+  <si>
+    <t>﻿1180120.875</t>
+  </si>
+  <si>
+    <t>﻿-26.89071455058124</t>
+  </si>
+  <si>
+    <t>﻿48484.12863525156</t>
+  </si>
+  <si>
+    <t>﻿-949134.25</t>
+  </si>
+  <si>
+    <t>﻿675807.5</t>
+  </si>
+  <si>
+    <t>﻿128.3882951996776</t>
+  </si>
+  <si>
+    <t>﻿20189.49938279508</t>
+  </si>
+  <si>
+    <t>﻿-773725.625</t>
+  </si>
+  <si>
+    <t>﻿891763.25</t>
+  </si>
+  <si>
+    <t>﻿155.2790139308098</t>
+  </si>
+  <si>
+    <t>﻿34726.0555352466</t>
+  </si>
+  <si>
+    <t>﻿-1029950.875</t>
+  </si>
+  <si>
+    <t>﻿894548.4375</t>
+  </si>
+  <si>
+    <t>﻿-4.859509287767654</t>
+  </si>
+  <si>
+    <t>﻿40353.3177984799</t>
+  </si>
+  <si>
+    <t>﻿-548113.9375</t>
+  </si>
+  <si>
+    <t>﻿456771.625</t>
+  </si>
+  <si>
+    <t>﻿229.3293888799148</t>
+  </si>
+  <si>
+    <t>﻿15611.21730743706</t>
+  </si>
+  <si>
+    <t>﻿-483699.625</t>
+  </si>
+  <si>
+    <t>﻿533721.25</t>
+  </si>
+  <si>
+    <t>﻿234.1889014477292</t>
+  </si>
+  <si>
+    <t>﻿29853.37261857623</t>
+  </si>
+  <si>
+    <t>﻿-1218061.5</t>
+  </si>
+  <si>
+    <t>﻿995438.5625</t>
+  </si>
+  <si>
+    <t>﻿21.80159882347294</t>
+  </si>
+  <si>
+    <t>﻿40265.26929741778</t>
+  </si>
+  <si>
+    <t>﻿-830920.625</t>
+  </si>
+  <si>
+    <t>﻿726528.125</t>
+  </si>
+  <si>
+    <t>﻿-68.95277914496262</t>
+  </si>
+  <si>
+    <t>﻿17128.33119944241</t>
+  </si>
+  <si>
+    <t>﻿-609494.8125</t>
+  </si>
+  <si>
+    <t>﻿551443.5625</t>
+  </si>
+  <si>
+    <t>﻿-90.75437709265925</t>
+  </si>
+  <si>
+    <t>﻿28788.04457327184</t>
+  </si>
+  <si>
+    <t>﻿-581158.375</t>
+  </si>
+  <si>
+    <t>﻿413679.125</t>
+  </si>
+  <si>
+    <t>﻿-2.489460189524948</t>
+  </si>
+  <si>
+    <t>﻿25145.9410290118</t>
+  </si>
+  <si>
+    <t>﻿-291865.3125</t>
+  </si>
+  <si>
+    <t>﻿260779.40625</t>
+  </si>
+  <si>
+    <t>﻿154.8795127016608</t>
+  </si>
+  <si>
+    <t>﻿10253.54669347173</t>
+  </si>
+  <si>
+    <t>﻿-251671.375</t>
+  </si>
+  <si>
+    <t>﻿289293.09375</t>
+  </si>
+  <si>
+    <t>﻿157.3689750197024</t>
+  </si>
+  <si>
+    <t>﻿18280.91224766725</t>
+  </si>
+  <si>
+    <t>﻿-484825.625</t>
+  </si>
+  <si>
+    <t>﻿404021.5</t>
+  </si>
+  <si>
+    <t>﻿-1.883414292423037</t>
+  </si>
+  <si>
+    <t>﻿22506.74222491689</t>
+  </si>
+  <si>
+    <t>﻿-318155.125</t>
+  </si>
+  <si>
+    <t>﻿222519.671875</t>
+  </si>
+  <si>
+    <t>﻿183.4667321760636</t>
+  </si>
+  <si>
+    <t>﻿8930.000367487199</t>
+  </si>
+  <si>
+    <t>﻿-222949.421875</t>
+  </si>
+  <si>
+    <t>﻿251741.09375</t>
+  </si>
+  <si>
+    <t>﻿185.3501443496111</t>
+  </si>
+  <si>
+    <t>﻿16549.66379897751</t>
+  </si>
+  <si>
+    <t>﻿-1193695.25</t>
+  </si>
+  <si>
+    <t>﻿827917.3125</t>
+  </si>
+  <si>
+    <t>﻿-13.30181260373695</t>
+  </si>
+  <si>
+    <t>﻿39237.52955074998</t>
+  </si>
+  <si>
+    <t>﻿-605731.1875</t>
+  </si>
+  <si>
+    <t>﻿660538.875</t>
+  </si>
+  <si>
+    <t>﻿51.29519074153393</t>
+  </si>
+  <si>
+    <t>﻿16751.06642110747</t>
+  </si>
+  <si>
+    <t>﻿-500761.0625</t>
+  </si>
+  <si>
+    <t>﻿587964.125</t>
+  </si>
+  <si>
+    <t>﻿64.59699784417192</t>
+  </si>
+  <si>
+    <t>﻿27839.1605116148</t>
+  </si>
+  <si>
+    <t>﻿-644506.1875</t>
+  </si>
+  <si>
+    <t>﻿1012788.5625</t>
+  </si>
+  <si>
+    <t>﻿21.3281337007885</t>
+  </si>
+  <si>
+    <t>﻿33490.01200894069</t>
+  </si>
+  <si>
+    <t>﻿-415213.46875</t>
+  </si>
+  <si>
+    <t>﻿464095.25</t>
+  </si>
+  <si>
+    <t>﻿106.7433467175595</t>
+  </si>
+  <si>
+    <t>﻿14231.75918874525</t>
+  </si>
+  <si>
+    <t>﻿-548693.25</t>
+  </si>
+  <si>
+    <t>﻿434067.4375</t>
+  </si>
+  <si>
+    <t>﻿85.4152145635036</t>
+  </si>
+  <si>
+    <t>﻿23639.81446106736</t>
+  </si>
+  <si>
+    <t>﻿-1068989.75</t>
+  </si>
+  <si>
+    <t>﻿1191166.125</t>
+  </si>
+  <si>
+    <t>﻿24.08350381246964</t>
+  </si>
+  <si>
+    <t>﻿40186.89274370919</t>
+  </si>
+  <si>
+    <t>﻿-684005.6875</t>
+  </si>
+  <si>
+    <t>﻿771900.5</t>
+  </si>
+  <si>
+    <t>﻿133.6739162886238</t>
+  </si>
+  <si>
+    <t>﻿18253.03856412928</t>
+  </si>
+  <si>
+    <t>﻿-560219.75</t>
+  </si>
+  <si>
+    <t>﻿470533.84375</t>
+  </si>
+  <si>
+    <t>﻿109.5904158386907</t>
+  </si>
+  <si>
+    <t>﻿27451.69706129897</t>
+  </si>
+  <si>
+    <t>﻿-695221.4375</t>
+  </si>
+  <si>
+    <t>﻿917453.5</t>
+  </si>
+  <si>
+    <t>﻿23.49199252291045</t>
+  </si>
+  <si>
+    <t>﻿28943.74895661767</t>
+  </si>
+  <si>
+    <t>﻿-357413</t>
+  </si>
+  <si>
+    <t>﻿612217.875</t>
+  </si>
+  <si>
+    <t>﻿133.0377693711821</t>
+  </si>
+  <si>
+    <t>﻿11333.18884435961</t>
+  </si>
+  <si>
+    <t>﻿-604190.75</t>
+  </si>
+  <si>
+    <t>﻿363408.75</t>
+  </si>
+  <si>
+    <t>﻿109.5457744649473</t>
+  </si>
+  <si>
+    <t>﻿21415.29122871073</t>
+  </si>
+  <si>
+    <t>﻿-1371410.625</t>
+  </si>
+  <si>
+    <t>﻿1016936.8125</t>
+  </si>
+  <si>
+    <t>﻿16.51513934175423</t>
+  </si>
+  <si>
+    <t>﻿47979.2108718057</t>
+  </si>
+  <si>
+    <t>﻿-688331.4375</t>
+  </si>
+  <si>
+    <t>﻿683380.8125</t>
+  </si>
+  <si>
+    <t>﻿92.60313476437791</t>
+  </si>
+  <si>
+    <t>﻿21113.80697604632</t>
+  </si>
+  <si>
+    <t>﻿-473871.96875</t>
+  </si>
+  <si>
+    <t>﻿683079.1875</t>
+  </si>
+  <si>
+    <t>﻿76.08800160310179</t>
+  </si>
+  <si>
+    <t>﻿33008.01395387486</t>
+  </si>
+  <si>
+    <t>﻿-1753387.875</t>
+  </si>
+  <si>
+    <t>﻿1206146.5</t>
+  </si>
+  <si>
+    <t>﻿20.03387626256952</t>
+  </si>
+  <si>
+    <t>﻿55551.0069204293</t>
+  </si>
+  <si>
+    <t>﻿-1199566.25</t>
+  </si>
+  <si>
+    <t>﻿605247.5625</t>
+  </si>
+  <si>
+    <t>﻿-180.0552967265203</t>
+  </si>
+  <si>
+    <t>﻿25221.8320191554</t>
+  </si>
+  <si>
+    <t>﻿-669846.0625</t>
+  </si>
+  <si>
+    <t>﻿1069074</t>
+  </si>
+  <si>
+    <t>﻿-200.0891635128051</t>
+  </si>
+  <si>
+    <t>﻿37946.09441479387</t>
+  </si>
+  <si>
+    <t>﻿-906321.5</t>
+  </si>
+  <si>
+    <t>﻿607348.6875</t>
+  </si>
+  <si>
+    <t>﻿6.857635687731429</t>
+  </si>
+  <si>
+    <t>﻿41844.37202340025</t>
+  </si>
+  <si>
+    <t>﻿-521451.28125</t>
+  </si>
+  <si>
+    <t>﻿392003.65625</t>
+  </si>
+  <si>
+    <t>﻿-235.5171235314416</t>
+  </si>
+  <si>
+    <t>﻿18760.4479572783</t>
+  </si>
+  <si>
+    <t>﻿-355475</t>
+  </si>
+  <si>
+    <t>﻿446582.71875</t>
+  </si>
+  <si>
+    <t>﻿-242.3747576740865</t>
+  </si>
+  <si>
+    <t>﻿29794.02915972369</t>
+  </si>
+  <si>
+    <t>﻿-1542052.25</t>
+  </si>
+  <si>
+    <t>﻿965467</t>
+  </si>
+  <si>
+    <t>﻿-8.512719032599948</t>
+  </si>
+  <si>
+    <t>﻿50406.54806140216</t>
+  </si>
+  <si>
+    <t>﻿-867381.25</t>
+  </si>
+  <si>
+    <t>﻿583818.4375</t>
+  </si>
+  <si>
+    <t>﻿-352.372175566256</t>
+  </si>
+  <si>
+    <t>﻿21605.17661898958</t>
+  </si>
+  <si>
+    <t>﻿-568927.8125</t>
+  </si>
+  <si>
+    <t>﻿674671.0625</t>
+  </si>
+  <si>
+    <t>﻿-343.8594623244506</t>
+  </si>
+  <si>
+    <t>﻿35149.24258419528</t>
+  </si>
+  <si>
+    <t>﻿-751854.6875</t>
+  </si>
+  <si>
+    <t>﻿717108.9375</t>
+  </si>
+  <si>
+    <t>﻿-26.53134540619528</t>
+  </si>
+  <si>
+    <t>﻿38335.5537370083</t>
+  </si>
+  <si>
+    <t>﻿-472035.1875</t>
+  </si>
+  <si>
+    <t>﻿438700.5</t>
+  </si>
+  <si>
+    <t>﻿-120.0848530435332</t>
+  </si>
+  <si>
+    <t>﻿19522.18229854034</t>
+  </si>
+  <si>
+    <t>﻿-322493.96875</t>
+  </si>
+  <si>
+    <t>﻿402634.78125</t>
+  </si>
+  <si>
+    <t>﻿-93.55350245328016</t>
+  </si>
+  <si>
+    <t>﻿25070.75084682268</t>
+  </si>
+  <si>
+    <t>﻿-566699.25</t>
+  </si>
+  <si>
+    <t>﻿581095.9375</t>
+  </si>
+  <si>
+    <t>﻿14.9987804002712</t>
+  </si>
+  <si>
+    <t>﻿23438.06967467201</t>
+  </si>
+  <si>
+    <t>﻿-262457.9375</t>
+  </si>
+  <si>
+    <t>﻿226155.234375</t>
+  </si>
+  <si>
+    <t>﻿60.8482253553608</t>
+  </si>
+  <si>
+    <t>﻿10284.01995939888</t>
+  </si>
+  <si>
+    <t>﻿-398582.46875</t>
+  </si>
+  <si>
+    <t>﻿304241.3125</t>
+  </si>
+  <si>
+    <t>﻿45.84944439960885</t>
+  </si>
+  <si>
+    <t>﻿16700.90643196355</t>
+  </si>
+  <si>
+    <t>﻿-1428914.5</t>
+  </si>
+  <si>
+    <t>﻿1652338.25</t>
+  </si>
+  <si>
+    <t>﻿-29.17123869861111</t>
+  </si>
+  <si>
+    <t>﻿56334.63369980814</t>
+  </si>
+  <si>
+    <t>﻿-961145.1875</t>
+  </si>
+  <si>
+    <t>﻿905570</t>
+  </si>
+  <si>
+    <t>﻿-229.9629347318459</t>
+  </si>
+  <si>
+    <t>﻿27618.69486279353</t>
+  </si>
+  <si>
+    <t>﻿-785179.6875</t>
+  </si>
+  <si>
+    <t>﻿808391.75</t>
+  </si>
+  <si>
+    <t>﻿-200.791692958447</t>
+  </si>
+  <si>
+    <t>﻿36281.6299119637</t>
+  </si>
+  <si>
+    <t>﻿-416582.09375</t>
+  </si>
+  <si>
+    <t>﻿367425.6875</t>
+  </si>
+  <si>
+    <t>﻿17.83071730652719</t>
+  </si>
+  <si>
+    <t>﻿21954.79255944594</t>
+  </si>
+  <si>
+    <t>﻿-280085.65625</t>
+  </si>
+  <si>
+    <t>﻿259741.6875</t>
+  </si>
+  <si>
+    <t>﻿111.6201454520034</t>
+  </si>
+  <si>
+    <t>﻿8880.35302117599</t>
+  </si>
+  <si>
+    <t>﻿-235900.9375</t>
+  </si>
+  <si>
+    <t>﻿243811.765625</t>
+  </si>
+  <si>
+    <t>﻿93.78942948740504</t>
+  </si>
+  <si>
+    <t>﻿16606.35383728476</t>
   </si>
 </sst>
 </file>
@@ -608,21 +1448,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:15" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,8 +1498,20 @@
       <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -685,8 +1542,20 @@
       <c r="J2">
         <v>41838.255903999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="L2" t="s">
+        <v>222</v>
+      </c>
+      <c r="M2" t="s">
+        <v>223</v>
+      </c>
+      <c r="N2" t="s">
+        <v>224</v>
+      </c>
+      <c r="O2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -717,8 +1586,20 @@
       <c r="J3">
         <v>50403.860889000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="L3" t="s">
+        <v>234</v>
+      </c>
+      <c r="M3" t="s">
+        <v>235</v>
+      </c>
+      <c r="N3" t="s">
+        <v>236</v>
+      </c>
+      <c r="O3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -749,8 +1630,20 @@
       <c r="J4">
         <v>38361.877787999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4" t="s">
+        <v>246</v>
+      </c>
+      <c r="M4" t="s">
+        <v>247</v>
+      </c>
+      <c r="N4" t="s">
+        <v>248</v>
+      </c>
+      <c r="O4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -781,8 +1674,20 @@
       <c r="J5">
         <v>23446.006163999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5" t="s">
+        <v>258</v>
+      </c>
+      <c r="M5" t="s">
+        <v>259</v>
+      </c>
+      <c r="N5" t="s">
+        <v>260</v>
+      </c>
+      <c r="O5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -813,8 +1718,20 @@
       <c r="J6">
         <v>56366.002074000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="L6" t="s">
+        <v>270</v>
+      </c>
+      <c r="M6" t="s">
+        <v>271</v>
+      </c>
+      <c r="N6" t="s">
+        <v>272</v>
+      </c>
+      <c r="O6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -845,8 +1762,20 @@
       <c r="J7">
         <v>21957.674724</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="L7" t="s">
+        <v>282</v>
+      </c>
+      <c r="M7" t="s">
+        <v>283</v>
+      </c>
+      <c r="N7" t="s">
+        <v>284</v>
+      </c>
+      <c r="O7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -877,8 +1806,20 @@
       <c r="J8">
         <v>72399.535954000006</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -909,8 +1850,20 @@
       <c r="J9">
         <v>71806.889941999994</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="L9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -941,8 +1894,20 @@
       <c r="J10">
         <v>32156.272868</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="L10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -973,8 +1938,20 @@
       <c r="J11">
         <v>26487.705945000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="L11" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1005,8 +1982,20 @@
       <c r="J12">
         <v>21791.173404000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1037,8 +2026,20 @@
       <c r="J13">
         <v>136742.12552999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="L13" t="s">
+        <v>78</v>
+      </c>
+      <c r="M13" t="s">
+        <v>79</v>
+      </c>
+      <c r="N13" t="s">
+        <v>80</v>
+      </c>
+      <c r="O13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1069,8 +2070,20 @@
       <c r="J14">
         <v>48490.080484999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="L14" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" t="s">
+        <v>91</v>
+      </c>
+      <c r="N14" t="s">
+        <v>92</v>
+      </c>
+      <c r="O14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1101,8 +2114,20 @@
       <c r="J15">
         <v>40349.908405000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="L15" t="s">
+        <v>102</v>
+      </c>
+      <c r="M15" t="s">
+        <v>103</v>
+      </c>
+      <c r="N15" t="s">
+        <v>104</v>
+      </c>
+      <c r="O15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1133,8 +2158,20 @@
       <c r="J16">
         <v>40244.563208</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="L16" t="s">
+        <v>114</v>
+      </c>
+      <c r="M16" t="s">
+        <v>115</v>
+      </c>
+      <c r="N16" t="s">
+        <v>116</v>
+      </c>
+      <c r="O16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1165,8 +2202,20 @@
       <c r="J17">
         <v>25144.194873</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="L17" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" t="s">
+        <v>127</v>
+      </c>
+      <c r="N17" t="s">
+        <v>128</v>
+      </c>
+      <c r="O17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1197,8 +2246,20 @@
       <c r="J18">
         <v>22543.819511999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="L18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M18" t="s">
+        <v>139</v>
+      </c>
+      <c r="N18" t="s">
+        <v>140</v>
+      </c>
+      <c r="O18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1229,8 +2290,20 @@
       <c r="J19">
         <v>39218.805068000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="L19" t="s">
+        <v>150</v>
+      </c>
+      <c r="M19" t="s">
+        <v>151</v>
+      </c>
+      <c r="N19" t="s">
+        <v>152</v>
+      </c>
+      <c r="O19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1261,8 +2334,20 @@
       <c r="J20">
         <v>33495.219247000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="L20" t="s">
+        <v>162</v>
+      </c>
+      <c r="M20" t="s">
+        <v>163</v>
+      </c>
+      <c r="N20" t="s">
+        <v>164</v>
+      </c>
+      <c r="O20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1293,8 +2378,20 @@
       <c r="J21">
         <v>40179.384750999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="L21" t="s">
+        <v>174</v>
+      </c>
+      <c r="M21" t="s">
+        <v>175</v>
+      </c>
+      <c r="N21" t="s">
+        <v>176</v>
+      </c>
+      <c r="O21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1325,8 +2422,20 @@
       <c r="J22">
         <v>28921.363394</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="L22" t="s">
+        <v>186</v>
+      </c>
+      <c r="M22" t="s">
+        <v>187</v>
+      </c>
+      <c r="N22" t="s">
+        <v>188</v>
+      </c>
+      <c r="O22" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1357,8 +2466,20 @@
       <c r="J23">
         <v>47951.082281000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="L23" t="s">
+        <v>198</v>
+      </c>
+      <c r="M23" t="s">
+        <v>199</v>
+      </c>
+      <c r="N23" t="s">
+        <v>200</v>
+      </c>
+      <c r="O23" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1388,6 +2509,18 @@
       </c>
       <c r="J24">
         <v>55525.653897999997</v>
+      </c>
+      <c r="L24" t="s">
+        <v>210</v>
+      </c>
+      <c r="M24" t="s">
+        <v>211</v>
+      </c>
+      <c r="N24" t="s">
+        <v>212</v>
+      </c>
+      <c r="O24" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1403,21 +2536,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:15" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1448,8 +2586,20 @@
       <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1480,8 +2630,20 @@
       <c r="J2">
         <v>18762.238883000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="L2" t="s">
+        <v>226</v>
+      </c>
+      <c r="M2" t="s">
+        <v>227</v>
+      </c>
+      <c r="N2" t="s">
+        <v>228</v>
+      </c>
+      <c r="O2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1512,8 +2674,20 @@
       <c r="J3">
         <v>21603.622876000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="L3" t="s">
+        <v>238</v>
+      </c>
+      <c r="M3" t="s">
+        <v>239</v>
+      </c>
+      <c r="N3" t="s">
+        <v>240</v>
+      </c>
+      <c r="O3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1544,8 +2718,20 @@
       <c r="J4">
         <v>19540.174029000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4" t="s">
+        <v>250</v>
+      </c>
+      <c r="M4" t="s">
+        <v>251</v>
+      </c>
+      <c r="N4" t="s">
+        <v>252</v>
+      </c>
+      <c r="O4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1576,8 +2762,20 @@
       <c r="J5">
         <v>10288.875067000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5" t="s">
+        <v>262</v>
+      </c>
+      <c r="M5" t="s">
+        <v>263</v>
+      </c>
+      <c r="N5" t="s">
+        <v>264</v>
+      </c>
+      <c r="O5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1608,8 +2806,20 @@
       <c r="J6">
         <v>27638.879755000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="L6" t="s">
+        <v>274</v>
+      </c>
+      <c r="M6" t="s">
+        <v>275</v>
+      </c>
+      <c r="N6" t="s">
+        <v>276</v>
+      </c>
+      <c r="O6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1640,8 +2850,20 @@
       <c r="J7">
         <v>8882.0834919999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="L7" t="s">
+        <v>286</v>
+      </c>
+      <c r="M7" t="s">
+        <v>287</v>
+      </c>
+      <c r="N7" t="s">
+        <v>288</v>
+      </c>
+      <c r="O7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1672,8 +2894,20 @@
       <c r="J8">
         <v>33391.594806000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="L8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1704,8 +2938,20 @@
       <c r="J9">
         <v>31851.100923999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1736,8 +2982,20 @@
       <c r="J10">
         <v>12834.099646999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="L10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1768,8 +3026,20 @@
       <c r="J11">
         <v>9837.8624120000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="L11" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" t="s">
+        <v>59</v>
+      </c>
+      <c r="N11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1800,8 +3070,20 @@
       <c r="J12">
         <v>8169.9046719999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="L12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N12" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1832,8 +3114,20 @@
       <c r="J13">
         <v>70832.989560999995</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="L13" t="s">
+        <v>82</v>
+      </c>
+      <c r="M13" t="s">
+        <v>83</v>
+      </c>
+      <c r="N13" t="s">
+        <v>84</v>
+      </c>
+      <c r="O13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1864,8 +3158,20 @@
       <c r="J14">
         <v>20190.334466</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="L14" t="s">
+        <v>94</v>
+      </c>
+      <c r="M14" t="s">
+        <v>95</v>
+      </c>
+      <c r="N14" t="s">
+        <v>96</v>
+      </c>
+      <c r="O14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1896,8 +3202,20 @@
       <c r="J15">
         <v>15615.651464</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="L15" t="s">
+        <v>106</v>
+      </c>
+      <c r="M15" t="s">
+        <v>107</v>
+      </c>
+      <c r="N15" t="s">
+        <v>108</v>
+      </c>
+      <c r="O15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1928,8 +3246,20 @@
       <c r="J16">
         <v>17108.019038999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="L16" t="s">
+        <v>118</v>
+      </c>
+      <c r="M16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N16" t="s">
+        <v>120</v>
+      </c>
+      <c r="O16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1960,8 +3290,20 @@
       <c r="J17">
         <v>10253.25049</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="L17" t="s">
+        <v>130</v>
+      </c>
+      <c r="M17" t="s">
+        <v>131</v>
+      </c>
+      <c r="N17" t="s">
+        <v>132</v>
+      </c>
+      <c r="O17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1992,8 +3334,20 @@
       <c r="J18">
         <v>8946.3652750000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="L18" t="s">
+        <v>142</v>
+      </c>
+      <c r="M18" t="s">
+        <v>143</v>
+      </c>
+      <c r="N18" t="s">
+        <v>144</v>
+      </c>
+      <c r="O18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2024,8 +3378,20 @@
       <c r="J19">
         <v>16757.179501999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="L19" t="s">
+        <v>154</v>
+      </c>
+      <c r="M19" t="s">
+        <v>155</v>
+      </c>
+      <c r="N19" t="s">
+        <v>156</v>
+      </c>
+      <c r="O19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2056,8 +3422,20 @@
       <c r="J20">
         <v>14234.795894000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="L20" t="s">
+        <v>166</v>
+      </c>
+      <c r="M20" t="s">
+        <v>167</v>
+      </c>
+      <c r="N20" t="s">
+        <v>168</v>
+      </c>
+      <c r="O20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2088,8 +3466,20 @@
       <c r="J21">
         <v>18250.686593999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="L21" t="s">
+        <v>178</v>
+      </c>
+      <c r="M21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N21" t="s">
+        <v>180</v>
+      </c>
+      <c r="O21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2120,8 +3510,20 @@
       <c r="J22">
         <v>11332.558585000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="L22" t="s">
+        <v>190</v>
+      </c>
+      <c r="M22" t="s">
+        <v>191</v>
+      </c>
+      <c r="N22" t="s">
+        <v>192</v>
+      </c>
+      <c r="O22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2152,8 +3554,20 @@
       <c r="J23">
         <v>21115.616704</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="L23" t="s">
+        <v>202</v>
+      </c>
+      <c r="M23" t="s">
+        <v>203</v>
+      </c>
+      <c r="N23" t="s">
+        <v>204</v>
+      </c>
+      <c r="O23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2183,6 +3597,18 @@
       </c>
       <c r="J24">
         <v>25211.843893000001</v>
+      </c>
+      <c r="L24" t="s">
+        <v>214</v>
+      </c>
+      <c r="M24" t="s">
+        <v>215</v>
+      </c>
+      <c r="N24" t="s">
+        <v>216</v>
+      </c>
+      <c r="O24" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2198,21 +3624,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:15" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2243,8 +3674,20 @@
       <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2275,8 +3718,20 @@
       <c r="J2">
         <v>29781.615046999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="L2" t="s">
+        <v>230</v>
+      </c>
+      <c r="M2" t="s">
+        <v>231</v>
+      </c>
+      <c r="N2" t="s">
+        <v>232</v>
+      </c>
+      <c r="O2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2307,8 +3762,20 @@
       <c r="J3">
         <v>35147.673825999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="L3" t="s">
+        <v>242</v>
+      </c>
+      <c r="M3" t="s">
+        <v>243</v>
+      </c>
+      <c r="N3" t="s">
+        <v>244</v>
+      </c>
+      <c r="O3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2339,8 +3806,20 @@
       <c r="J4">
         <v>25075.772999000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4" t="s">
+        <v>254</v>
+      </c>
+      <c r="M4" t="s">
+        <v>255</v>
+      </c>
+      <c r="N4" t="s">
+        <v>256</v>
+      </c>
+      <c r="O4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2371,8 +3850,20 @@
       <c r="J5">
         <v>16703.246536999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5" t="s">
+        <v>266</v>
+      </c>
+      <c r="M5" t="s">
+        <v>267</v>
+      </c>
+      <c r="N5" t="s">
+        <v>268</v>
+      </c>
+      <c r="O5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2403,8 +3894,20 @@
       <c r="J6">
         <v>36299.224089000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="L6" t="s">
+        <v>278</v>
+      </c>
+      <c r="M6" t="s">
+        <v>279</v>
+      </c>
+      <c r="N6" t="s">
+        <v>280</v>
+      </c>
+      <c r="O6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2435,8 +3938,20 @@
       <c r="J7">
         <v>16608.315945999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="L7" t="s">
+        <v>290</v>
+      </c>
+      <c r="M7" t="s">
+        <v>291</v>
+      </c>
+      <c r="N7" t="s">
+        <v>292</v>
+      </c>
+      <c r="O7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2467,8 +3982,20 @@
       <c r="J8">
         <v>48310.521367000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="L8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2499,8 +4026,20 @@
       <c r="J9">
         <v>47876.026595000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="L9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2531,8 +4070,20 @@
       <c r="J10">
         <v>23505.292346999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="L10" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" t="s">
+        <v>51</v>
+      </c>
+      <c r="N10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2563,8 +4114,20 @@
       <c r="J11">
         <v>19999.705773000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="L11" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" t="s">
+        <v>63</v>
+      </c>
+      <c r="N11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2595,8 +4158,20 @@
       <c r="J12">
         <v>16397.700195000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="L12" t="s">
+        <v>74</v>
+      </c>
+      <c r="M12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12" t="s">
+        <v>76</v>
+      </c>
+      <c r="O12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2627,8 +4202,20 @@
       <c r="J13">
         <v>81325.228357</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="L13" t="s">
+        <v>86</v>
+      </c>
+      <c r="M13" t="s">
+        <v>87</v>
+      </c>
+      <c r="N13" t="s">
+        <v>88</v>
+      </c>
+      <c r="O13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2659,8 +4246,20 @@
       <c r="J14">
         <v>34731.985918999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="L14" t="s">
+        <v>98</v>
+      </c>
+      <c r="M14" t="s">
+        <v>99</v>
+      </c>
+      <c r="N14" t="s">
+        <v>100</v>
+      </c>
+      <c r="O14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -2691,8 +4290,20 @@
       <c r="J15">
         <v>29842.102578000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="L15" t="s">
+        <v>110</v>
+      </c>
+      <c r="M15" t="s">
+        <v>111</v>
+      </c>
+      <c r="N15" t="s">
+        <v>112</v>
+      </c>
+      <c r="O15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2723,8 +4334,20 @@
       <c r="J16">
         <v>28786.213066</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="L16" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16" t="s">
+        <v>123</v>
+      </c>
+      <c r="N16" t="s">
+        <v>124</v>
+      </c>
+      <c r="O16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2755,8 +4378,20 @@
       <c r="J17">
         <v>18279.826574999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="L17" t="s">
+        <v>134</v>
+      </c>
+      <c r="M17" t="s">
+        <v>135</v>
+      </c>
+      <c r="N17" t="s">
+        <v>136</v>
+      </c>
+      <c r="O17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -2787,8 +4422,20 @@
       <c r="J18">
         <v>16572.217178999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="L18" t="s">
+        <v>146</v>
+      </c>
+      <c r="M18" t="s">
+        <v>147</v>
+      </c>
+      <c r="N18" t="s">
+        <v>148</v>
+      </c>
+      <c r="O18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2819,8 +4466,20 @@
       <c r="J19">
         <v>27800.070318999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="L19" t="s">
+        <v>158</v>
+      </c>
+      <c r="M19" t="s">
+        <v>159</v>
+      </c>
+      <c r="N19" t="s">
+        <v>160</v>
+      </c>
+      <c r="O19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2851,8 +4510,20 @@
       <c r="J20">
         <v>23643.288209999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="L20" t="s">
+        <v>170</v>
+      </c>
+      <c r="M20" t="s">
+        <v>171</v>
+      </c>
+      <c r="N20" t="s">
+        <v>172</v>
+      </c>
+      <c r="O20" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2883,8 +4554,20 @@
       <c r="J21">
         <v>27445.876854999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="L21" t="s">
+        <v>182</v>
+      </c>
+      <c r="M21" t="s">
+        <v>183</v>
+      </c>
+      <c r="N21" t="s">
+        <v>184</v>
+      </c>
+      <c r="O21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2915,8 +4598,20 @@
       <c r="J22">
         <v>21393.328504000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="L22" t="s">
+        <v>194</v>
+      </c>
+      <c r="M22" t="s">
+        <v>195</v>
+      </c>
+      <c r="N22" t="s">
+        <v>196</v>
+      </c>
+      <c r="O22" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2947,8 +4642,20 @@
       <c r="J23">
         <v>32973.437319999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="L23" t="s">
+        <v>206</v>
+      </c>
+      <c r="M23" t="s">
+        <v>207</v>
+      </c>
+      <c r="N23" t="s">
+        <v>208</v>
+      </c>
+      <c r="O23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2978,6 +4685,18 @@
       </c>
       <c r="J24">
         <v>37925.557688000001</v>
+      </c>
+      <c r="L24" t="s">
+        <v>218</v>
+      </c>
+      <c r="M24" t="s">
+        <v>219</v>
+      </c>
+      <c r="N24" t="s">
+        <v>220</v>
+      </c>
+      <c r="O24" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>